<commit_message>
add consent for pns in hts initial form. change icon for forms to show file icon. correct concept for other cadre in linkage form
</commit_message>
<xml_diff>
--- a/config/default/forms/contact/patient_contact-create.xlsx
+++ b/config/default/forms/contact/patient_contact-create.xlsx
@@ -2911,124 +2911,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="28">
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <font>
         <name val="Arial"/>
@@ -3240,25 +3123,25 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="B47" activeCellId="0" sqref="B47"/>
+      <selection pane="bottomRight" activeCell="C47" activeCellId="0" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.8673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.719387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="104.484693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.9285714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="77.2142857142857"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="64.8877551020408"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="147.678571428571"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.719387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="49.5867346938776"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="27.719387755102"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="58.9438775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="27.719387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0969387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.8775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.6683673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.7091836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="108.265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.0969387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="79.9132653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="67.2244897959184"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="152.989795918367"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="28.7091836734694"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="51.2959183673469"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="28.7091836734694"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="61.015306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="28.7091836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4370,7 +4253,7 @@
         <v>121</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
@@ -5460,375 +5343,375 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A64">
-    <cfRule type="cellIs" priority="105" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="cellIs" priority="105" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H64">
-    <cfRule type="expression" priority="106" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="106" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND(NOT($G64 = ""), $H64 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E64">
-    <cfRule type="expression" priority="107" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="expression" priority="107" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A64="begin repeat", NOT($B64 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E64">
-    <cfRule type="expression" priority="108" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="expression" priority="108" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($E64 = "", $A64 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E64">
-    <cfRule type="expression" priority="109" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="expression" priority="109" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A64="end repeat", $B64 = "", $C64 = "", $D64 = "", $E64 = "", $F64 = "", $G64 = "", $H64 = "", $E64 = "", $J64 = "", $K64 = "", $L64 = "", $M64 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E64">
-    <cfRule type="expression" priority="110" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="expression" priority="110" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A64="end group", $B64 = "", $C64 = "", $D64 = "", $E64 = "", $F64 = "", $G64 = "", $H64 = "", $E64 = "", $J64 = "", $K64 = "", $L64 = "", $M64 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E64">
-    <cfRule type="containsText" priority="111" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="5"/>
+    <cfRule type="containsText" priority="111" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" priority="112" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="112" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($C17 = "", $A17 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" priority="113" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="113" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A17="end repeat", $B17 = "", $C17 = "", $D17 = "", $E17 = "", $F17 = "", $G17 = "", $H17 = "", $C17 = "", $J17 = "", $K17 = "", $L17 = "", $M17 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" priority="114" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="114" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A17="end group", $B17 = "", $C17 = "", $D17 = "", $E17 = "", $F17 = "", $G17 = "", $H17 = "", $C17 = "", $J17 = "", $K17 = "", $L17 = "", $M17 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56">
-    <cfRule type="containsText" priority="115" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="7"/>
+    <cfRule type="containsText" priority="115" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56">
-    <cfRule type="expression" priority="116" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="116" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A56="begin group", NOT($B56 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56">
-    <cfRule type="expression" priority="117" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="117" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A56="end group", $B56 = "", $C56 = "", $D56 = "", $E56 = "", $F56 = "", $G56 = "", $H56 = "", $I56 = "", $J56 = "", $K56 = "", $L56 = "", $M56 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56">
-    <cfRule type="cellIs" priority="118" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="cellIs" priority="118" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56">
-    <cfRule type="cellIs" priority="119" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="cellIs" priority="119" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56">
-    <cfRule type="expression" priority="120" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="120" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A56="begin repeat", NOT($B56 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56">
-    <cfRule type="expression" priority="121" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="121" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A56="end repeat", $B56 = "", $C56 = "", $D56 = "", $E56 = "", $F56 = "", $G56 = "", $H56 = "", $I56 = "", $J56 = "", $K56 = "", $L56 = "", $M56 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B56">
-    <cfRule type="containsText" priority="122" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="7"/>
+    <cfRule type="containsText" priority="122" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B56">
-    <cfRule type="expression" priority="123" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="123" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A56="begin group", NOT($B56 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B56">
-    <cfRule type="expression" priority="124" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="124" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A56="end group", $B56 = "", $C56 = "", $D56 = "", $E56 = "", $F56 = "", $G56 = "", $H56 = "", $I56 = "", $J56 = "", $K56 = "", $L56 = "", $M56 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B56">
-    <cfRule type="cellIs" priority="125" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="cellIs" priority="125" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B56">
-    <cfRule type="expression" priority="126" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="126" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(AND(NOT($A56 = "end group"), NOT($A56 = "end repeat"), NOT($A56 = "")), $B56 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B56">
-    <cfRule type="expression" priority="127" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="127" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A56="begin repeat", NOT($B56 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B56">
-    <cfRule type="expression" priority="128" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="128" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A56="end repeat", $B56 = "", $C56 = "", $D56 = "", $E56 = "", $F56 = "", $G56 = "", $H56 = "", $I56 = "", $J56 = "", $K56 = "", $L56 = "", $M56 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B56">
-    <cfRule type="expression" priority="129" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="129" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>COUNTIF($B$2:$B$1069,B56)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56">
-    <cfRule type="containsText" priority="130" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="7"/>
+    <cfRule type="containsText" priority="130" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56">
-    <cfRule type="expression" priority="131" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="131" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A56="begin group", NOT($B56 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56">
-    <cfRule type="expression" priority="132" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="132" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A56="end group", $B56 = "", $C56 = "", $D56 = "", $E56 = "", $F56 = "", $G56 = "", $H56 = "", $I56 = "", $J56 = "", $K56 = "", $L56 = "", $M56 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56">
-    <cfRule type="cellIs" priority="133" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="133" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56">
-    <cfRule type="expression" priority="134" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="134" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A56="begin repeat", NOT($B56 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56">
-    <cfRule type="expression" priority="135" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="135" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A56="end repeat", $B56 = "", $C56 = "", $D56 = "", $E56 = "", $F56 = "", $G56 = "", $H56 = "", $I56 = "", $J56 = "", $K56 = "", $L56 = "", $M56 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E57">
-    <cfRule type="containsText" priority="136" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="12"/>
+    <cfRule type="containsText" priority="136" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E57">
-    <cfRule type="expression" priority="137" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="137" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A57="begin group", NOT($B57 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E57">
-    <cfRule type="expression" priority="138" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="expression" priority="138" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A57="end group", $B57 = "", $C57 = "", $D57 = "", $E57 = "", $F57 = "", $G57 = "", $H57 = "", $I57 = "", $J57 = "", $K57 = "", $L57 = "", $M57 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E57">
-    <cfRule type="cellIs" priority="139" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="cellIs" priority="139" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E57">
-    <cfRule type="expression" priority="140" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="expression" priority="140" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A57="begin repeat", NOT($B57 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E57">
-    <cfRule type="expression" priority="141" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="expression" priority="141" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A57="end repeat", $B57 = "", $C57 = "", $D57 = "", $E57 = "", $F57 = "", $G57 = "", $H57 = "", $I57 = "", $J57 = "", $K57 = "", $L57 = "", $M57 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58">
-    <cfRule type="cellIs" priority="142" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="cellIs" priority="142" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E58">
-    <cfRule type="containsText" priority="143" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="13"/>
+    <cfRule type="containsText" priority="143" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E58">
-    <cfRule type="expression" priority="144" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="expression" priority="144" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A58="begin group", NOT($B58 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E58">
-    <cfRule type="expression" priority="145" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="expression" priority="145" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A58="end group", $B58 = "", $C58 = "", $D58 = "", $E58 = "", $F58 = "", $G58 = "", $H58 = "", $I58 = "", $J58 = "", $K58 = "", $L58 = "", $M58 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E58">
-    <cfRule type="cellIs" priority="146" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="cellIs" priority="146" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E58">
-    <cfRule type="expression" priority="147" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="expression" priority="147" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A58="begin repeat", NOT($B58 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E58">
-    <cfRule type="expression" priority="148" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="expression" priority="148" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A58="end repeat", $B58 = "", $C58 = "", $D58 = "", $E58 = "", $F58 = "", $G58 = "", $H58 = "", $I58 = "", $J58 = "", $K58 = "", $L58 = "", $M58 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="containsText" priority="149" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="13"/>
+    <cfRule type="containsText" priority="149" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="cellIs" priority="150" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="cellIs" priority="150" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="containsText" priority="151" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="13"/>
+    <cfRule type="containsText" priority="151" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="cellIs" priority="152" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="cellIs" priority="152" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="containsText" priority="153" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="13"/>
+    <cfRule type="containsText" priority="153" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="cellIs" priority="154" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="cellIs" priority="154" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="containsText" priority="155" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="14"/>
+    <cfRule type="containsText" priority="155" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="cellIs" priority="156" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+    <cfRule type="cellIs" priority="156" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="expression" priority="157" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
+    <cfRule type="expression" priority="157" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>AND(A1 = "type", COUNTIF($A$1:$A$923, "begin group") = COUNTIF($A$1:$A$923, "end group"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="expression" priority="158" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
+    <cfRule type="expression" priority="158" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>OR(NOT(A1 = "type"), NOT(COUNTIF($A$1:$A$914, "begin group") = COUNTIF($A$1:$A$923, "end group")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="expression" priority="159" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
+    <cfRule type="expression" priority="159" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>AND($A43="begin repeat", NOT($B43 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="expression" priority="160" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
+    <cfRule type="expression" priority="160" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>AND($A43="end repeat", $B43 = "", $C43 = "", $D43 = "", $E43 = "", $F43 = "", $G43 = "", $H43 = "", $I43 = "", $J43 = "", $K43 = "", $L43 = "", $M43 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="expression" priority="161" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
+    <cfRule type="expression" priority="161" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>AND($A43="end group", $B43 = "", $C43 = "", $D43 = "", $E43 = "", $F43 = "", $G43 = "", $H43 = "", $I43 = "", $J43 = "", $K43 = "", $L43 = "", $M43 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="expression" priority="162" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
+    <cfRule type="expression" priority="162" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>AND($A43="begin group", NOT($B43 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="containsText" priority="163" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="15"/>
+    <cfRule type="containsText" priority="163" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="cellIs" priority="164" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+    <cfRule type="cellIs" priority="164" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="containsText" priority="165" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="16"/>
+    <cfRule type="containsText" priority="165" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="cellIs" priority="166" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+    <cfRule type="cellIs" priority="166" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43">
-    <cfRule type="cellIs" priority="167" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+    <cfRule type="cellIs" priority="167" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="containsText" priority="168" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="17"/>
+    <cfRule type="containsText" priority="168" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="cellIs" priority="169" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
+    <cfRule type="cellIs" priority="169" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42">
-    <cfRule type="containsText" priority="170" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="13"/>
+    <cfRule type="containsText" priority="170" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42">
-    <cfRule type="cellIs" priority="171" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="cellIs" priority="171" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42">
-    <cfRule type="containsText" priority="172" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="13"/>
+    <cfRule type="containsText" priority="172" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42">
-    <cfRule type="cellIs" priority="173" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="cellIs" priority="173" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:N8">
-    <cfRule type="containsText" priority="174" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="19"/>
+    <cfRule type="containsText" priority="174" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:N8">
-    <cfRule type="expression" priority="175" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20">
+    <cfRule type="expression" priority="175" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A7="begin group", NOT($B7 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:N8">
-    <cfRule type="expression" priority="176" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
+    <cfRule type="expression" priority="176" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($A7="end group", $B7 = "", $C7 = "", $D7 = "", $E7 = "", $F7 = "", $G7 = "", $H7 = "", $I7 = "", $J7 = "", $K7 = "", $L7 = "", $M7 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:N8">
-    <cfRule type="cellIs" priority="177" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22">
+    <cfRule type="cellIs" priority="177" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:I8">
-    <cfRule type="expression" priority="178" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23">
+    <cfRule type="expression" priority="178" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND($I7 = "", $A7 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:C8">
-    <cfRule type="expression" priority="179" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24">
+    <cfRule type="expression" priority="179" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>AND(AND(NOT($A7 = "end group"), NOT($A7 = "end repeat"), NOT($A7 = "")), $C7 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:B8">
-    <cfRule type="expression" priority="180" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25">
+    <cfRule type="expression" priority="180" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>AND(AND(NOT(#ref! = "end group"), NOT(#ref! = "end repeat"), NOT(#ref! = "")), #ref! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:A8">
-    <cfRule type="cellIs" priority="181" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26">
+    <cfRule type="cellIs" priority="181" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:H8">
-    <cfRule type="expression" priority="182" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26">
+    <cfRule type="expression" priority="182" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
       <formula>AND(NOT(#ref! = ""), #ref! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:N8">
-    <cfRule type="expression" priority="183" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27">
+    <cfRule type="expression" priority="183" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
       <formula>AND($A7="begin repeat", NOT($B7 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:N8">
-    <cfRule type="expression" priority="184" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27">
+    <cfRule type="expression" priority="184" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
       <formula>AND($A7="end repeat", $B7 = "", $C7 = "", $D7 = "", $E7 = "", $F7 = "", $G7 = "", $H7 = "", $I7 = "", $J7 = "", $K7 = "", $L7 = "", $M7 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:B8">
-    <cfRule type="expression" priority="185" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27">
+    <cfRule type="expression" priority="185" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
       <formula>COUNTIF($B$2:$B$991,#ref!)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5867,10 +5750,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.219387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.4642857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="77.8469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="27.719387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.6275510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="80.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="28.7091836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -27045,9 +26928,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="27.719387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.1785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="27.719387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="28.7091836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="28.7091836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -27082,7 +26965,7 @@
       </c>
       <c r="C2" s="36" t="n">
         <f aca="true">NOW()</f>
-        <v>44293.6264326682</v>
+        <v>44294.4156812803</v>
       </c>
       <c r="D2" s="28" t="s">
         <v>843</v>

</xml_diff>